<commit_message>
update a few fields
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-05-08.xlsx
+++ b/EC/Train Runs and Enforcements 2016-05-08.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wabtec\Documents\GitHub\eaglep3\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stu\Documents\GitHub\eaglep3-reporting\EC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Enforcements!$A$2:$N$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Train Runs'!$A$2:$AA$2</definedName>
-    <definedName name="Denver_Train_Runs_04122016" localSheetId="0">'Train Runs'!$A$2:$J$156</definedName>
+    <definedName name="Denver_Train_Runs_04122016" localSheetId="0">'Train Runs'!$A$2:$J$155</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="445">
   <si>
     <t>Train ID</t>
   </si>
@@ -1388,10 +1388,7 @@
     <t>Routing at DUS</t>
   </si>
   <si>
-    <t>Signal unspecified\unknown EC0508RH 43-1T 1N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crew Logoff </t>
+    <t>Brief comm outage due to comparator issue caused enforcement at EC0508RH 43-1T 1N</t>
   </si>
 </sst>
 </file>
@@ -1881,14 +1878,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -1897,100 +1887,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2025,110 +1927,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -2150,48 +1948,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2475,10 +2231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CK168"/>
+  <dimension ref="A1:CK167"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R151" sqref="R151"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A118" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9268,7 +9024,7 @@
         <v>2.7916666673263535E-2</v>
       </c>
       <c r="N81" s="13">
-        <f t="shared" ref="N81:P130" si="26">$M81*24*60</f>
+        <f t="shared" ref="N81:N130" si="26">$M81*24*60</f>
         <v>40.20000000949949</v>
       </c>
       <c r="O81" s="13"/>
@@ -12279,7 +12035,7 @@
         <v>0</v>
       </c>
       <c r="K117" s="61" t="str">
-        <f t="shared" ref="K117:K151" si="34">IF(ISEVEN(B117),(B117-1)&amp;"/"&amp;B117,B117&amp;"/"&amp;(B117+1))</f>
+        <f t="shared" ref="K117:K150" si="34">IF(ISEVEN(B117),(B117-1)&amp;"/"&amp;B117,B117&amp;"/"&amp;(B117+1))</f>
         <v>4017/4018</v>
       </c>
       <c r="L117" s="61" t="str">
@@ -12287,7 +12043,7 @@
         <v>STEWART</v>
       </c>
       <c r="M117" s="12">
-        <f t="shared" ref="M117:M151" si="35">I117-F117</f>
+        <f t="shared" ref="M117:M150" si="35">I117-F117</f>
         <v>2.6180555556493346E-2</v>
       </c>
       <c r="N117" s="13">
@@ -14643,7 +14399,7 @@
         <v>3.8958333330811001E-2</v>
       </c>
       <c r="N145" s="13">
-        <f t="shared" ref="N145:N151" si="38">$M145*24*60</f>
+        <f t="shared" ref="N145:N150" si="38">$M145*24*60</f>
         <v>56.099999996367842</v>
       </c>
       <c r="O145" s="13"/>
@@ -14987,27 +14743,27 @@
       <c r="Q149" s="62"/>
       <c r="R149" s="62"/>
       <c r="T149" s="75" t="str">
-        <f t="shared" ref="T149:T151" si="44">"https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'"&amp;TEXT(E149-1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600',mode:absolute,to:'"&amp;TEXT(I149+1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed',"&amp;"'Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:"&amp;"(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc."&amp;B149&amp;"%22')),sort:!(Time,asc))"</f>
+        <f t="shared" ref="T149:T150" si="44">"https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'"&amp;TEXT(E149-1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600',mode:absolute,to:'"&amp;TEXT(I149+1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed',"&amp;"'Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:"&amp;"(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc."&amp;B149&amp;"%22')),sort:!(Time,asc))"</f>
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-05-09 00:10:50-0600',mode:absolute,to:'2016-05-09 01:08:01-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4029%22')),sort:!(Time,asc))</v>
       </c>
       <c r="U149" s="75" t="str">
-        <f t="shared" ref="U149:U151" si="45">IF(Y149&lt;23,"Y","N")</f>
+        <f t="shared" ref="U149:U150" si="45">IF(Y149&lt;23,"Y","N")</f>
         <v>N</v>
       </c>
       <c r="V149" s="75">
-        <f t="shared" ref="V149:V151" si="46">VALUE(LEFT(A149,3))-VALUE(LEFT(A148,3))</f>
+        <f t="shared" ref="V149:V150" si="46">VALUE(LEFT(A149,3))-VALUE(LEFT(A148,3))</f>
         <v>1</v>
       </c>
       <c r="W149" s="75">
-        <f t="shared" ref="W149:W151" si="47">RIGHT(D149,LEN(D149)-4)/10000</f>
+        <f t="shared" ref="W149:W150" si="47">RIGHT(D149,LEN(D149)-4)/10000</f>
         <v>4.7100000000000003E-2</v>
       </c>
       <c r="X149" s="75">
-        <f t="shared" ref="X149:X151" si="48">RIGHT(H149,LEN(H149)-4)/10000</f>
+        <f t="shared" ref="X149:X150" si="48">RIGHT(H149,LEN(H149)-4)/10000</f>
         <v>23.310400000000001</v>
       </c>
       <c r="Y149" s="75">
-        <f t="shared" ref="Y149:Y151" si="49">ABS(X149-W149)</f>
+        <f t="shared" ref="Y149:Y150" si="49">ABS(X149-W149)</f>
         <v>23.263300000000001</v>
       </c>
       <c r="Z149" s="76" t="e">
@@ -15103,136 +14859,81 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="151" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="61" t="s">
-        <v>403</v>
-      </c>
-      <c r="B151" s="61">
-        <v>4020</v>
-      </c>
-      <c r="C151" s="61" t="s">
-        <v>83</v>
-      </c>
-      <c r="D151" s="61" t="s">
-        <v>268</v>
-      </c>
-      <c r="E151" s="30">
-        <v>42499.049189814818</v>
-      </c>
-      <c r="F151" s="30">
-        <v>42499.050509259258</v>
-      </c>
-      <c r="G151" s="38">
-        <v>1</v>
-      </c>
-      <c r="H151" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="I151" s="30">
-        <v>42499.050509259258</v>
-      </c>
-      <c r="J151" s="61">
-        <v>0</v>
-      </c>
-      <c r="K151" s="61" t="str">
-        <f t="shared" si="34"/>
-        <v>4019/4020</v>
-      </c>
-      <c r="L151" s="61" t="str">
-        <f>VLOOKUP(A151,'Trips&amp;Operators'!$C$1:$E$9999,3,FALSE)</f>
-        <v>YOUNG</v>
-      </c>
-      <c r="M151" s="12">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="N151" s="13"/>
-      <c r="O151" s="13"/>
-      <c r="P151" s="13">
-        <v>1</v>
-      </c>
-      <c r="Q151" s="62"/>
-      <c r="R151" s="62" t="s">
-        <v>445</v>
-      </c>
-      <c r="T151" s="75" t="str">
-        <f t="shared" si="44"/>
-        <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-05-09 01:09:50-0600',mode:absolute,to:'2016-05-09 01:13:44-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4020%22')),sort:!(Time,asc))</v>
-      </c>
-      <c r="U151" s="75" t="str">
-        <f t="shared" si="45"/>
-        <v>Y</v>
-      </c>
-      <c r="V151" s="75">
-        <f t="shared" si="46"/>
-        <v>67</v>
-      </c>
-      <c r="W151" s="75">
-        <f t="shared" si="47"/>
-        <v>4.6199999999999998E-2</v>
-      </c>
-      <c r="X151" s="75">
-        <f t="shared" si="48"/>
-        <v>4.6199999999999998E-2</v>
-      </c>
-      <c r="Y151" s="75">
-        <f t="shared" si="49"/>
-        <v>0</v>
-      </c>
-      <c r="Z151" s="76" t="e">
-        <f>VLOOKUP(A151,Enforcements!$C$3:$J$26,8,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA151" s="76" t="e">
-        <f>VLOOKUP(A151,Enforcements!$C$3:$J$26,3,0)</f>
-        <v>#N/A</v>
-      </c>
+    <row r="151" spans="1:27" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="64"/>
+      <c r="B151" s="64"/>
+      <c r="C151" s="64"/>
+      <c r="D151" s="64"/>
+      <c r="E151" s="65"/>
+      <c r="F151" s="65"/>
+      <c r="G151" s="66"/>
+      <c r="H151" s="65"/>
+      <c r="I151" s="65"/>
+      <c r="J151" s="64"/>
+      <c r="K151" s="64"/>
+      <c r="L151" s="64"/>
+      <c r="M151" s="67"/>
+      <c r="N151" s="68"/>
+      <c r="O151" s="68"/>
+      <c r="P151" s="68"/>
+      <c r="Q151" s="69"/>
+      <c r="R151" s="69"/>
+      <c r="T151" s="70"/>
+      <c r="U151" s="70"/>
+      <c r="V151" s="70"/>
+      <c r="W151" s="70"/>
+      <c r="X151" s="70"/>
+      <c r="Y151" s="70"/>
+      <c r="Z151" s="71"/>
+      <c r="AA151" s="71"/>
     </row>
     <row r="152" spans="1:27" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="64"/>
-      <c r="B152" s="64"/>
-      <c r="C152" s="64"/>
-      <c r="D152" s="64"/>
-      <c r="E152" s="65"/>
-      <c r="F152" s="65"/>
-      <c r="G152" s="66"/>
-      <c r="H152" s="65"/>
-      <c r="I152" s="65"/>
-      <c r="J152" s="64"/>
-      <c r="K152" s="64"/>
-      <c r="L152" s="64"/>
-      <c r="M152" s="67"/>
-      <c r="N152" s="68"/>
-      <c r="O152" s="68"/>
-      <c r="P152" s="68"/>
-      <c r="Q152" s="69"/>
-      <c r="R152" s="69"/>
-      <c r="T152" s="70"/>
-      <c r="U152" s="70"/>
-      <c r="V152" s="70"/>
-      <c r="W152" s="70"/>
-      <c r="X152" s="70"/>
-      <c r="Y152" s="70"/>
-      <c r="Z152" s="71"/>
-      <c r="AA152" s="71"/>
+      <c r="E152" s="31"/>
+      <c r="F152" s="31"/>
+      <c r="G152" s="39"/>
+      <c r="H152" s="31"/>
+      <c r="I152" s="78">
+        <f>Variables!A2</f>
+        <v>42495</v>
+      </c>
+      <c r="J152" s="79"/>
+      <c r="K152" s="77"/>
+      <c r="L152" s="77"/>
+      <c r="M152" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="N152" s="81"/>
+      <c r="O152" s="82"/>
+      <c r="P152" s="5"/>
+      <c r="T152" s="57"/>
+      <c r="U152" s="57"/>
+      <c r="V152" s="57"/>
+      <c r="W152" s="57"/>
+      <c r="X152" s="57"/>
+      <c r="Y152" s="57"/>
+      <c r="Z152" s="58"/>
+      <c r="AA152" s="58"/>
     </row>
     <row r="153" spans="1:27" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E153" s="31"/>
       <c r="F153" s="31"/>
       <c r="G153" s="39"/>
       <c r="H153" s="31"/>
-      <c r="I153" s="78">
-        <f>Variables!A2</f>
-        <v>42495</v>
-      </c>
-      <c r="J153" s="79"/>
-      <c r="K153" s="77"/>
-      <c r="L153" s="77"/>
-      <c r="M153" s="80" t="s">
-        <v>8</v>
-      </c>
-      <c r="N153" s="81"/>
-      <c r="O153" s="82"/>
+      <c r="I153" s="83" t="s">
+        <v>10</v>
+      </c>
+      <c r="J153" s="84"/>
+      <c r="K153" s="35"/>
+      <c r="L153" s="59"/>
+      <c r="M153" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N153" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O153" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="P153" s="5"/>
       <c r="T153" s="57"/>
       <c r="U153" s="57"/>
@@ -15248,20 +14949,23 @@
       <c r="F154" s="31"/>
       <c r="G154" s="39"/>
       <c r="H154" s="31"/>
-      <c r="I154" s="83" t="s">
-        <v>10</v>
-      </c>
-      <c r="J154" s="84"/>
-      <c r="K154" s="35"/>
-      <c r="L154" s="59"/>
-      <c r="M154" s="9" t="s">
-        <v>11</v>
+      <c r="I154" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="J154" s="3">
+        <f>COUNT(N3:P150)</f>
+        <v>145</v>
+      </c>
+      <c r="K154" s="3"/>
+      <c r="L154" s="3"/>
+      <c r="M154" s="72" t="s">
+        <v>15</v>
       </c>
       <c r="N154" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O154" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P154" s="5"/>
       <c r="T154" s="57"/>
@@ -15279,22 +14983,25 @@
       <c r="G155" s="39"/>
       <c r="H155" s="31"/>
       <c r="I155" s="32" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J155" s="3">
-        <f>COUNT(N3:P151)</f>
-        <v>146</v>
+        <f>COUNT(N3:N150)</f>
+        <v>137</v>
       </c>
       <c r="K155" s="3"/>
       <c r="L155" s="3"/>
-      <c r="M155" s="72" t="s">
-        <v>15</v>
-      </c>
-      <c r="N155" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="O155" s="7" t="s">
-        <v>15</v>
+      <c r="M155" s="72">
+        <f>AVERAGE(N3:N148)</f>
+        <v>43.162345679525608</v>
+      </c>
+      <c r="N155" s="6">
+        <f>MIN(N3:N150)</f>
+        <v>34.999999998835847</v>
+      </c>
+      <c r="O155" s="7">
+        <f>MAX(N3:N150)</f>
+        <v>57.783333335537463</v>
       </c>
       <c r="P155" s="5"/>
       <c r="T155" s="57"/>
@@ -15307,40 +15014,46 @@
       <c r="AA155" s="58"/>
     </row>
     <row r="156" spans="1:27" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E156" s="31"/>
-      <c r="F156" s="31"/>
-      <c r="G156" s="39"/>
-      <c r="H156" s="31"/>
-      <c r="I156" s="32" t="s">
-        <v>17</v>
+      <c r="B156"/>
+      <c r="C156"/>
+      <c r="D156"/>
+      <c r="E156" s="14"/>
+      <c r="F156" s="14"/>
+      <c r="G156" s="40"/>
+      <c r="H156" s="14"/>
+      <c r="I156" s="33" t="s">
+        <v>45</v>
       </c>
       <c r="J156" s="3">
-        <f>COUNT(N3:N151)</f>
-        <v>137</v>
+        <f>COUNT(O3:O150)</f>
+        <v>0</v>
       </c>
       <c r="K156" s="3"/>
       <c r="L156" s="3"/>
       <c r="M156" s="72">
-        <f>AVERAGE(N3:N148)</f>
-        <v>43.162345679525608</v>
+        <f>IFERROR(AVERAGE(O3:O150),0)</f>
+        <v>0</v>
       </c>
       <c r="N156" s="6">
-        <f>MIN(N3:N151)</f>
-        <v>34.999999998835847</v>
+        <f>MIN(O3:O148)</f>
+        <v>0</v>
       </c>
       <c r="O156" s="7">
-        <f>MAX(N3:N151)</f>
-        <v>57.783333335537463</v>
-      </c>
-      <c r="P156" s="5"/>
-      <c r="T156" s="57"/>
-      <c r="U156" s="57"/>
-      <c r="V156" s="57"/>
-      <c r="W156" s="57"/>
-      <c r="X156" s="57"/>
-      <c r="Y156" s="57"/>
-      <c r="Z156" s="58"/>
-      <c r="AA156" s="58"/>
+        <f>MAX(O3:O148)</f>
+        <v>0</v>
+      </c>
+      <c r="P156" s="4"/>
+      <c r="Q156"/>
+      <c r="R156"/>
+      <c r="S156"/>
+      <c r="T156" s="55"/>
+      <c r="U156" s="55"/>
+      <c r="V156" s="55"/>
+      <c r="W156" s="55"/>
+      <c r="X156" s="55"/>
+      <c r="Y156" s="55"/>
+      <c r="Z156" s="56"/>
+      <c r="AA156" s="56"/>
     </row>
     <row r="157" spans="1:27" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157"/>
@@ -15350,26 +15063,23 @@
       <c r="F157" s="14"/>
       <c r="G157" s="40"/>
       <c r="H157" s="14"/>
-      <c r="I157" s="33" t="s">
-        <v>45</v>
+      <c r="I157" s="34" t="s">
+        <v>9</v>
       </c>
       <c r="J157" s="3">
-        <f>COUNT(O3:O151)</f>
-        <v>0</v>
+        <f>COUNT(P3:P150)</f>
+        <v>8</v>
       </c>
       <c r="K157" s="3"/>
       <c r="L157" s="3"/>
-      <c r="M157" s="72">
-        <f>IFERROR(AVERAGE(O3:O151),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N157" s="6">
-        <f>MIN(O3:O148)</f>
-        <v>0</v>
-      </c>
-      <c r="O157" s="7">
-        <f>MAX(O3:O148)</f>
-        <v>0</v>
+      <c r="M157" s="72" t="s">
+        <v>15</v>
+      </c>
+      <c r="N157" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O157" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="P157" s="4"/>
       <c r="Q157"/>
@@ -15384,82 +15094,76 @@
       <c r="Z157" s="56"/>
       <c r="AA157" s="56"/>
     </row>
-    <row r="158" spans="1:27" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B158"/>
-      <c r="C158"/>
-      <c r="D158"/>
-      <c r="E158" s="14"/>
-      <c r="F158" s="14"/>
-      <c r="G158" s="40"/>
-      <c r="H158" s="14"/>
-      <c r="I158" s="34" t="s">
-        <v>9</v>
+    <row r="158" spans="1:27" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E158" s="31"/>
+      <c r="F158" s="31"/>
+      <c r="G158" s="39"/>
+      <c r="H158" s="31"/>
+      <c r="I158" s="32" t="s">
+        <v>16</v>
       </c>
       <c r="J158" s="3">
-        <f>COUNT(P3:P151)</f>
-        <v>9</v>
+        <f>COUNT(N3:O150)</f>
+        <v>137</v>
       </c>
       <c r="K158" s="3"/>
       <c r="L158" s="3"/>
-      <c r="M158" s="72" t="s">
-        <v>15</v>
-      </c>
-      <c r="N158" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="O158" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="P158" s="4"/>
-      <c r="Q158"/>
-      <c r="R158"/>
-      <c r="S158"/>
-      <c r="T158" s="55"/>
-      <c r="U158" s="55"/>
-      <c r="V158" s="55"/>
-      <c r="W158" s="55"/>
-      <c r="X158" s="55"/>
-      <c r="Y158" s="55"/>
-      <c r="Z158" s="56"/>
-      <c r="AA158" s="56"/>
+      <c r="M158" s="72">
+        <f>AVERAGE(N3:P150)</f>
+        <v>42.282068966026038</v>
+      </c>
+      <c r="N158" s="6">
+        <f>MIN(N3:O150)</f>
+        <v>34.999999998835847</v>
+      </c>
+      <c r="O158" s="7">
+        <f>MAX(N3:O150)</f>
+        <v>57.783333335537463</v>
+      </c>
+      <c r="P158" s="5"/>
+      <c r="T158" s="57"/>
+      <c r="U158" s="57"/>
+      <c r="V158" s="57"/>
+      <c r="W158" s="57"/>
+      <c r="X158" s="57"/>
+      <c r="Y158" s="57"/>
+      <c r="Z158" s="58"/>
+      <c r="AA158" s="58"/>
     </row>
     <row r="159" spans="1:27" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E159" s="31"/>
-      <c r="F159" s="31"/>
-      <c r="G159" s="39"/>
-      <c r="H159" s="31"/>
+      <c r="B159"/>
+      <c r="C159"/>
+      <c r="D159"/>
+      <c r="E159" s="14"/>
+      <c r="F159" s="14"/>
+      <c r="G159" s="40"/>
+      <c r="H159" s="14"/>
       <c r="I159" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="J159" s="3">
-        <f>COUNT(N3:O151)</f>
-        <v>137</v>
-      </c>
-      <c r="K159" s="3"/>
-      <c r="L159" s="3"/>
-      <c r="M159" s="72">
-        <f>AVERAGE(N3:P151)</f>
-        <v>41.999315068998463</v>
-      </c>
-      <c r="N159" s="6">
-        <f>MIN(N3:O151)</f>
-        <v>34.999999998835847</v>
-      </c>
-      <c r="O159" s="7">
-        <f>MAX(N3:O151)</f>
-        <v>57.783333335537463</v>
-      </c>
-      <c r="P159" s="5"/>
-      <c r="T159" s="57"/>
-      <c r="U159" s="57"/>
-      <c r="V159" s="57"/>
-      <c r="W159" s="57"/>
-      <c r="X159" s="57"/>
-      <c r="Y159" s="57"/>
-      <c r="Z159" s="58"/>
-      <c r="AA159" s="58"/>
-    </row>
-    <row r="160" spans="1:27" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="J159" s="8">
+        <f>J158/J154</f>
+        <v>0.94482758620689655</v>
+      </c>
+      <c r="K159" s="8"/>
+      <c r="L159" s="8"/>
+      <c r="M159" s="1"/>
+      <c r="N159" s="4"/>
+      <c r="O159" s="4"/>
+      <c r="P159" s="4"/>
+      <c r="Q159"/>
+      <c r="R159"/>
+      <c r="S159"/>
+      <c r="T159" s="55"/>
+      <c r="U159" s="55"/>
+      <c r="V159" s="55"/>
+      <c r="W159" s="55"/>
+      <c r="X159" s="55"/>
+      <c r="Y159" s="55"/>
+      <c r="Z159" s="56"/>
+      <c r="AA159" s="56"/>
+    </row>
+    <row r="160" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B160"/>
       <c r="C160"/>
       <c r="D160"/>
@@ -15467,15 +15171,10 @@
       <c r="F160" s="14"/>
       <c r="G160" s="40"/>
       <c r="H160" s="14"/>
-      <c r="I160" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="J160" s="8">
-        <f>J159/J155</f>
-        <v>0.93835616438356162</v>
-      </c>
-      <c r="K160" s="8"/>
-      <c r="L160" s="8"/>
+      <c r="I160" s="14"/>
+      <c r="J160"/>
+      <c r="K160"/>
+      <c r="L160" s="60"/>
       <c r="M160" s="1"/>
       <c r="N160" s="4"/>
       <c r="O160" s="4"/>
@@ -15604,104 +15303,68 @@
       <c r="Z164" s="56"/>
       <c r="AA164" s="56"/>
     </row>
-    <row r="165" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B165"/>
-      <c r="C165"/>
-      <c r="D165"/>
-      <c r="E165" s="14"/>
-      <c r="F165" s="14"/>
-      <c r="G165" s="40"/>
-      <c r="H165" s="14"/>
-      <c r="I165" s="14"/>
-      <c r="J165"/>
-      <c r="K165"/>
-      <c r="L165" s="60"/>
-      <c r="M165" s="1"/>
-      <c r="N165" s="4"/>
-      <c r="O165" s="4"/>
-      <c r="P165" s="4"/>
-      <c r="Q165"/>
-      <c r="R165"/>
-      <c r="S165"/>
-      <c r="T165" s="55"/>
-      <c r="U165" s="55"/>
-      <c r="V165" s="55"/>
-      <c r="W165" s="55"/>
-      <c r="X165" s="55"/>
-      <c r="Y165" s="55"/>
-      <c r="Z165" s="56"/>
-      <c r="AA165" s="56"/>
-    </row>
-    <row r="168" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B168"/>
-      <c r="C168"/>
-      <c r="D168"/>
-      <c r="E168" s="14"/>
-      <c r="F168" s="14"/>
-      <c r="G168" s="40"/>
-      <c r="H168" s="14"/>
-      <c r="I168" s="14"/>
-      <c r="J168"/>
-      <c r="K168"/>
-      <c r="L168" s="60"/>
-      <c r="M168" s="1"/>
-      <c r="N168" s="4"/>
-      <c r="O168" s="4"/>
-      <c r="P168" s="4"/>
-      <c r="Q168"/>
-      <c r="R168"/>
-      <c r="S168"/>
-      <c r="T168" s="55"/>
-      <c r="U168" s="55"/>
-      <c r="V168" s="55"/>
-      <c r="W168" s="55"/>
-      <c r="X168" s="55"/>
-      <c r="Y168" s="55"/>
-      <c r="Z168" s="56"/>
-      <c r="AA168" s="56"/>
+    <row r="167" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B167"/>
+      <c r="C167"/>
+      <c r="D167"/>
+      <c r="E167" s="14"/>
+      <c r="F167" s="14"/>
+      <c r="G167" s="40"/>
+      <c r="H167" s="14"/>
+      <c r="I167" s="14"/>
+      <c r="J167"/>
+      <c r="K167"/>
+      <c r="L167" s="60"/>
+      <c r="M167" s="1"/>
+      <c r="N167" s="4"/>
+      <c r="O167" s="4"/>
+      <c r="P167" s="4"/>
+      <c r="Q167"/>
+      <c r="R167"/>
+      <c r="S167"/>
+      <c r="T167" s="55"/>
+      <c r="U167" s="55"/>
+      <c r="V167" s="55"/>
+      <c r="W167" s="55"/>
+      <c r="X167" s="55"/>
+      <c r="Y167" s="55"/>
+      <c r="Z167" s="56"/>
+      <c r="AA167" s="56"/>
     </row>
   </sheetData>
   <sortState ref="A3:Y144">
     <sortCondition ref="A3:A144"/>
   </sortState>
   <mergeCells count="4">
+    <mergeCell ref="I152:J152"/>
+    <mergeCell ref="M152:O152"/>
     <mergeCell ref="I153:J153"/>
-    <mergeCell ref="M153:O153"/>
-    <mergeCell ref="I154:J154"/>
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="U1:V1 U2 U3:V1048576">
-    <cfRule type="cellIs" dxfId="36" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="20" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1 V3:V1048576">
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L127:L151 A3:R148 A149:P152">
-    <cfRule type="expression" dxfId="34" priority="34">
+  <conditionalFormatting sqref="A3:R148 L127:L150 A149:P151">
+    <cfRule type="expression" dxfId="6" priority="34">
       <formula>$P3&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="35">
+    <cfRule type="expression" dxfId="5" priority="35">
       <formula>$O3&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q152:R152">
-    <cfRule type="expression" dxfId="31" priority="76">
-      <formula>$P152&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="77">
-      <formula>$O171&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="Q149:R151">
-    <cfRule type="expression" dxfId="29" priority="78">
+    <cfRule type="expression" dxfId="4" priority="76">
       <formula>$P149&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="79">
-      <formula>$O169&gt;0</formula>
+    <cfRule type="expression" dxfId="3" priority="77">
+      <formula>$O168&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15720,7 +15383,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A3:R152</xm:sqref>
+          <xm:sqref>A3:R151</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -17988,12 +17651,12 @@
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="N2 M2:M1048576">
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:N52">
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$M3="Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add all redmine tickets for 5/8
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-05-08.xlsx
+++ b/EC/Train Runs and Enforcements 2016-05-08.xlsx
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Enforcements!$A$2:$N$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Train Runs'!$A$2:$AA$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Train Runs'!$A$2:$AA$150</definedName>
     <definedName name="Denver_Train_Runs_04122016" localSheetId="0">'Train Runs'!$A$2:$J$155</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="446">
   <si>
     <t>Train ID</t>
   </si>
@@ -1388,7 +1388,10 @@
     <t>Routing at DUS</t>
   </si>
   <si>
-    <t>Brief comm outage due to comparator issue caused enforcement at EC0508RH 43-1T 1N</t>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Comm outage due to comparator issue caused red fence at EC0508RH 43-1T 1N. Ran in ATC for remainder of trip</t>
   </si>
 </sst>
 </file>
@@ -2233,8 +2236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CK167"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A118" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R95" sqref="R95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3819,7 +3822,9 @@
         <f t="shared" si="2"/>
         <v>35.899999999674037</v>
       </c>
-      <c r="Q19" s="62"/>
+      <c r="Q19" s="62" t="s">
+        <v>444</v>
+      </c>
       <c r="R19" s="62" t="s">
         <v>441</v>
       </c>
@@ -4041,7 +4046,7 @@
         <v>42498.280972222223</v>
       </c>
       <c r="F22" s="30">
-        <v>42498.28634259259</v>
+        <v>42498.289212962962</v>
       </c>
       <c r="G22" s="38">
         <v>7</v>
@@ -4050,7 +4055,7 @@
         <v>225</v>
       </c>
       <c r="I22" s="30">
-        <v>42498.290949074071</v>
+        <v>42498.313784722224</v>
       </c>
       <c r="J22" s="61">
         <v>0</v>
@@ -4065,25 +4070,23 @@
       </c>
       <c r="M22" s="12">
         <f t="shared" si="14"/>
-        <v>4.6064814814599231E-3</v>
-      </c>
-      <c r="N22" s="13"/>
+        <v>2.457175926247146E-2</v>
+      </c>
+      <c r="N22" s="13">
+        <f t="shared" si="2"/>
+        <v>35.383333337958902</v>
+      </c>
       <c r="O22" s="13"/>
-      <c r="P22" s="13">
-        <f t="shared" si="2"/>
-        <v>6.6333333333022892</v>
-      </c>
+      <c r="P22" s="13"/>
       <c r="Q22" s="62"/>
-      <c r="R22" s="62" t="s">
-        <v>442</v>
-      </c>
+      <c r="R22" s="62"/>
       <c r="T22" s="75" t="str">
         <f t="shared" si="15"/>
-        <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-05-08 06:43:36-0600',mode:absolute,to:'2016-05-08 06:59:58-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4039%22')),sort:!(Time,asc))</v>
+        <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-05-08 06:43:36-0600',mode:absolute,to:'2016-05-08 07:32:51-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4039%22')),sort:!(Time,asc))</v>
       </c>
       <c r="U22" s="75" t="str">
         <f t="shared" si="16"/>
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="V22" s="75">
         <f t="shared" si="17"/>
@@ -4094,12 +4097,11 @@
         <v>23.2971</v>
       </c>
       <c r="X22" s="75">
-        <f t="shared" si="19"/>
-        <v>22.387899999999998</v>
+        <v>0.19209999999999999</v>
       </c>
       <c r="Y22" s="75">
         <f t="shared" si="20"/>
-        <v>0.90920000000000201</v>
+        <v>23.105</v>
       </c>
       <c r="Z22" s="76" t="e">
         <f>VLOOKUP(A22,Enforcements!$C$3:$J$26,8,0)</f>
@@ -4242,7 +4244,9 @@
       <c r="P24" s="13">
         <v>43</v>
       </c>
-      <c r="Q24" s="62"/>
+      <c r="Q24" s="62" t="s">
+        <v>444</v>
+      </c>
       <c r="R24" s="62" t="s">
         <v>438</v>
       </c>
@@ -4912,7 +4916,9 @@
       <c r="P32" s="13">
         <v>42</v>
       </c>
-      <c r="Q32" s="62"/>
+      <c r="Q32" s="62" t="s">
+        <v>444</v>
+      </c>
       <c r="R32" s="62" t="s">
         <v>443</v>
       </c>
@@ -5414,7 +5420,9 @@
       <c r="P38" s="13">
         <v>1</v>
       </c>
-      <c r="Q38" s="62"/>
+      <c r="Q38" s="62" t="s">
+        <v>444</v>
+      </c>
       <c r="R38" s="62" t="s">
         <v>442</v>
       </c>
@@ -6507,7 +6515,9 @@
       <c r="P51" s="13">
         <v>15</v>
       </c>
-      <c r="Q51" s="62"/>
+      <c r="Q51" s="62" t="s">
+        <v>444</v>
+      </c>
       <c r="R51" s="62" t="s">
         <v>442</v>
       </c>
@@ -10204,9 +10214,11 @@
       <c r="P95" s="13">
         <v>49</v>
       </c>
-      <c r="Q95" s="62"/>
+      <c r="Q95" s="62" t="s">
+        <v>444</v>
+      </c>
       <c r="R95" s="62" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="T95" s="75" t="str">
         <f t="shared" si="27"/>
@@ -11126,7 +11138,9 @@
       <c r="P106" s="13">
         <v>10</v>
       </c>
-      <c r="Q106" s="62"/>
+      <c r="Q106" s="62" t="s">
+        <v>444</v>
+      </c>
       <c r="R106" s="62" t="s">
         <v>442</v>
       </c>
@@ -14987,13 +15001,13 @@
       </c>
       <c r="J155" s="3">
         <f>COUNT(N3:N150)</f>
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K155" s="3"/>
       <c r="L155" s="3"/>
       <c r="M155" s="72">
         <f>AVERAGE(N3:N148)</f>
-        <v>43.162345679525608</v>
+        <v>43.105147059367027</v>
       </c>
       <c r="N155" s="6">
         <f>MIN(N3:N150)</f>
@@ -15068,7 +15082,7 @@
       </c>
       <c r="J157" s="3">
         <f>COUNT(P3:P150)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K157" s="3"/>
       <c r="L157" s="3"/>
@@ -15104,13 +15118,13 @@
       </c>
       <c r="J158" s="3">
         <f>COUNT(N3:O150)</f>
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K158" s="3"/>
       <c r="L158" s="3"/>
       <c r="M158" s="72">
         <f>AVERAGE(N3:P150)</f>
-        <v>42.282068966026038</v>
+        <v>42.480344828127123</v>
       </c>
       <c r="N158" s="6">
         <f>MIN(N3:O150)</f>
@@ -15143,7 +15157,7 @@
       </c>
       <c r="J159" s="8">
         <f>J158/J154</f>
-        <v>0.94482758620689655</v>
+        <v>0.9517241379310345</v>
       </c>
       <c r="K159" s="8"/>
       <c r="L159" s="8"/>
@@ -15332,6 +15346,7 @@
       <c r="AA167" s="56"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:AA150"/>
   <sortState ref="A3:Y144">
     <sortCondition ref="A3:A144"/>
   </sortState>
@@ -15351,7 +15366,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:R148 L127:L150 A149:P151">
+  <conditionalFormatting sqref="L127:L150 A149:P151 A3:R148">
     <cfRule type="expression" dxfId="6" priority="34">
       <formula>$P3&gt;0</formula>
     </cfRule>

</xml_diff>